<commit_message>
fixed all gene knockouts
</commit_message>
<xml_diff>
--- a/input/Kampik_2021_mutants.xlsx
+++ b/input/Kampik_2021_mutants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idunmariaburgos/Documents/Work/Project/Ruminiclostridium cellulolyticum part 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Daniel/git/Ruminiclostridium-cellullolyticum-model-final/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB96F4BC-38EC-2A41-BF12-A785AB20F727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B12309E-E66B-5C47-90F4-366171FB9789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{3E5A3820-E0E0-5B4F-87D3-01E6E804A0F5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="54">
   <si>
     <t>Mutant</t>
   </si>
@@ -191,6 +191,15 @@
   </si>
   <si>
     <t>NOTE: SOME HAVE ALMOST NO EFFECT (not accounted for)</t>
+  </si>
+  <si>
+    <t>MTL2109</t>
+  </si>
+  <si>
+    <t>Ccel_2109</t>
+  </si>
+  <si>
+    <t>From Fosses 2017</t>
   </si>
 </sst>
 </file>
@@ -357,20 +366,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -394,9 +399,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -434,7 +439,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -540,7 +545,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -682,7 +687,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -690,13 +695,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACFA2D52-DE4C-0348-845A-3C8517871A18}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="27.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -726,38 +734,35 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
         <v>11</v>
       </c>
       <c r="I3" t="s">
@@ -765,36 +770,53 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
-        <v>10</v>
+      <c r="F4" t="s">
+        <v>11</v>
       </c>
       <c r="I4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -823,10 +845,10 @@
       <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="10" t="s">
         <v>20</v>
       </c>
       <c r="F1" t="s">
@@ -849,10 +871,10 @@
       <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G2" t="s">
@@ -861,355 +883,345 @@
       <c r="H2" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="13" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="7"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="9"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="12" t="s">
+      <c r="G5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="13"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="9"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="7"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="9"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="12" t="s">
+      <c r="G8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="13"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="6" t="s">
+      <c r="G9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="7"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="9"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="9"/>
+      <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="10"/>
+      <c r="E12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="6" t="s">
+      <c r="G12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="7"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="9"/>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="12" t="s">
+      <c r="G14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="13"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>